<commit_message>
Adding Comments in Your Code
</commit_message>
<xml_diff>
--- a/me/2.Apex-Fundamentals.xlsx
+++ b/me/2.Apex-Fundamentals.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDFEA3D-3069-4FA7-BA1F-C69CAB557A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123926AF-2D6F-4BFE-B277-BDBC178B353E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hello World" sheetId="1" r:id="rId1"/>
     <sheet name="Primitive Data Types" sheetId="2" r:id="rId2"/>
     <sheet name="String Class Methods" sheetId="3" r:id="rId3"/>
     <sheet name="Escape Character" sheetId="4" r:id="rId4"/>
+    <sheet name="Adding Comments" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
   <si>
     <t>Mở Developer Console trên tab mới</t>
   </si>
@@ -334,6 +335,60 @@
   </si>
   <si>
     <t>System.debug(str);</t>
+  </si>
+  <si>
+    <t>5.adding-comments.txt</t>
+  </si>
+  <si>
+    <t>salesforce\2.Apex-Fundamentals\5.adding-comments.txt</t>
+  </si>
+  <si>
+    <t>/* Adding multi-line comment</t>
+  </si>
+  <si>
+    <t>Long worldPopulation = 7000000000L;</t>
+  </si>
+  <si>
+    <t>Time currentTime = Time.newInstance(3, 25, 0, 0);</t>
+  </si>
+  <si>
+    <t>// get current date and time</t>
+  </si>
+  <si>
+    <t>*/</t>
+  </si>
+  <si>
+    <t>//adding single line comment</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comment 1 dòng: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comment nhiều dòng: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* */</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -462,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -483,9 +538,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2216,6 +2279,152 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>129181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5DD8278-D4EC-A777-8160-B86F9459995F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="8820150"/>
+          <a:ext cx="11382375" cy="5215531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>112826</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68801B13-3A4B-1FD8-C9E0-828780BA06AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="14239875"/>
+          <a:ext cx="11372850" cy="4922951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1C2983F-672B-98B1-939C-3107B6467915}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2352675" y="15849600"/>
+          <a:ext cx="457200" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5328,8 +5537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F5C844-989B-4063-8984-7E05E0019EFA}">
   <dimension ref="A3:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5350,47 +5559,37 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="14"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="14"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="14"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="14"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -5421,12 +5620,6 @@
       <c r="B15" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -5462,1178 +5655,226 @@
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
       <c r="T20" s="5"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
       <c r="T22" s="5"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
       <c r="T24" s="5"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
       <c r="T25" s="5"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
       <c r="T26" s="5"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
       <c r="T27" s="5"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
       <c r="T28" s="5"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
       <c r="T29" s="5"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
       <c r="T31" s="5"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
       <c r="T32" s="5"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
       <c r="T33" s="5"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
       <c r="T34" s="5"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
       <c r="T35" s="5"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
       <c r="T36" s="5"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
       <c r="T37" s="5"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
       <c r="T38" s="5"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
       <c r="T39" s="5"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
       <c r="T40" s="5"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
       <c r="T41" s="5"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
       <c r="T42" s="5"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
       <c r="T43" s="5"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
       <c r="T45" s="5"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
       <c r="T46" s="5"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
       <c r="T47" s="5"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
       <c r="T48" s="5"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
       <c r="T49" s="5"/>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="14"/>
       <c r="T50" s="5"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="14"/>
       <c r="T51" s="5"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
       <c r="T52" s="5"/>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
-      <c r="Q53" s="14"/>
-      <c r="R53" s="14"/>
-      <c r="S53" s="14"/>
       <c r="T53" s="5"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="14"/>
       <c r="T54" s="5"/>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="14"/>
       <c r="T55" s="5"/>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
-      <c r="O56" s="14"/>
-      <c r="P56" s="14"/>
-      <c r="Q56" s="14"/>
-      <c r="R56" s="14"/>
-      <c r="S56" s="14"/>
       <c r="T56" s="5"/>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
-      <c r="Q57" s="14"/>
-      <c r="R57" s="14"/>
-      <c r="S57" s="14"/>
       <c r="T57" s="5"/>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
-      <c r="N58" s="14"/>
-      <c r="O58" s="14"/>
-      <c r="P58" s="14"/>
-      <c r="Q58" s="14"/>
-      <c r="R58" s="14"/>
-      <c r="S58" s="14"/>
       <c r="T58" s="5"/>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
-      <c r="O59" s="14"/>
-      <c r="P59" s="14"/>
-      <c r="Q59" s="14"/>
-      <c r="R59" s="14"/>
-      <c r="S59" s="14"/>
       <c r="T59" s="5"/>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="14"/>
-      <c r="O60" s="14"/>
-      <c r="P60" s="14"/>
-      <c r="Q60" s="14"/>
-      <c r="R60" s="14"/>
-      <c r="S60" s="14"/>
       <c r="T60" s="5"/>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
-      <c r="L61" s="14"/>
-      <c r="M61" s="14"/>
-      <c r="N61" s="14"/>
-      <c r="O61" s="14"/>
-      <c r="P61" s="14"/>
-      <c r="Q61" s="14"/>
-      <c r="R61" s="14"/>
-      <c r="S61" s="14"/>
       <c r="T61" s="5"/>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="14"/>
-      <c r="N62" s="14"/>
-      <c r="O62" s="14"/>
-      <c r="P62" s="14"/>
-      <c r="Q62" s="14"/>
-      <c r="R62" s="14"/>
-      <c r="S62" s="14"/>
       <c r="T62" s="5"/>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="14"/>
-      <c r="O63" s="14"/>
-      <c r="P63" s="14"/>
-      <c r="Q63" s="14"/>
-      <c r="R63" s="14"/>
-      <c r="S63" s="14"/>
       <c r="T63" s="5"/>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="14"/>
-      <c r="O64" s="14"/>
-      <c r="P64" s="14"/>
-      <c r="Q64" s="14"/>
-      <c r="R64" s="14"/>
-      <c r="S64" s="14"/>
       <c r="T64" s="5"/>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-      <c r="O65" s="14"/>
-      <c r="P65" s="14"/>
-      <c r="Q65" s="14"/>
-      <c r="R65" s="14"/>
-      <c r="S65" s="14"/>
       <c r="T65" s="5"/>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14"/>
-      <c r="O66" s="14"/>
-      <c r="P66" s="14"/>
-      <c r="Q66" s="14"/>
-      <c r="R66" s="14"/>
-      <c r="S66" s="14"/>
       <c r="T66" s="5"/>
     </row>
     <row r="67" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
-      <c r="L67" s="14"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
-      <c r="O67" s="14"/>
-      <c r="P67" s="14"/>
-      <c r="Q67" s="14"/>
-      <c r="R67" s="14"/>
-      <c r="S67" s="14"/>
       <c r="T67" s="5"/>
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
-      <c r="O68" s="14"/>
-      <c r="P68" s="14"/>
-      <c r="Q68" s="14"/>
-      <c r="R68" s="14"/>
-      <c r="S68" s="14"/>
       <c r="T68" s="5"/>
     </row>
     <row r="69" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="14"/>
-      <c r="M69" s="14"/>
-      <c r="N69" s="14"/>
-      <c r="O69" s="14"/>
-      <c r="P69" s="14"/>
-      <c r="Q69" s="14"/>
-      <c r="R69" s="14"/>
-      <c r="S69" s="14"/>
       <c r="T69" s="5"/>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
-      <c r="M70" s="14"/>
-      <c r="N70" s="14"/>
-      <c r="O70" s="14"/>
-      <c r="P70" s="14"/>
-      <c r="Q70" s="14"/>
-      <c r="R70" s="14"/>
-      <c r="S70" s="14"/>
       <c r="T70" s="5"/>
     </row>
     <row r="71" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="14"/>
-      <c r="N71" s="14"/>
-      <c r="O71" s="14"/>
-      <c r="P71" s="14"/>
-      <c r="Q71" s="14"/>
-      <c r="R71" s="14"/>
-      <c r="S71" s="14"/>
       <c r="T71" s="5"/>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-      <c r="K72" s="14"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
-      <c r="O72" s="14"/>
-      <c r="P72" s="14"/>
-      <c r="Q72" s="14"/>
-      <c r="R72" s="14"/>
-      <c r="S72" s="14"/>
       <c r="T72" s="5"/>
     </row>
     <row r="73" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="L73" s="14"/>
-      <c r="M73" s="14"/>
-      <c r="N73" s="14"/>
-      <c r="O73" s="14"/>
-      <c r="P73" s="14"/>
-      <c r="Q73" s="14"/>
-      <c r="R73" s="14"/>
-      <c r="S73" s="14"/>
       <c r="T73" s="5"/>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14"/>
-      <c r="L74" s="14"/>
-      <c r="M74" s="14"/>
-      <c r="N74" s="14"/>
-      <c r="O74" s="14"/>
-      <c r="P74" s="14"/>
-      <c r="Q74" s="14"/>
-      <c r="R74" s="14"/>
-      <c r="S74" s="14"/>
       <c r="T74" s="5"/>
     </row>
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="14"/>
-      <c r="K75" s="14"/>
-      <c r="L75" s="14"/>
-      <c r="M75" s="14"/>
-      <c r="N75" s="14"/>
-      <c r="O75" s="14"/>
-      <c r="P75" s="14"/>
-      <c r="Q75" s="14"/>
-      <c r="R75" s="14"/>
-      <c r="S75" s="14"/>
       <c r="T75" s="5"/>
     </row>
     <row r="76" spans="2:20" x14ac:dyDescent="0.25">
@@ -6661,4 +5902,1677 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BB3148-3A03-489F-B349-9C98BD9F098C}">
+  <dimension ref="A2:T103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="8"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="3"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24"/>
+      <c r="K50" s="24"/>
+      <c r="L50" s="24"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="24"/>
+      <c r="O50" s="24"/>
+      <c r="P50" s="24"/>
+      <c r="Q50" s="24"/>
+      <c r="R50" s="24"/>
+      <c r="S50" s="24"/>
+      <c r="T50" s="5"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
+      <c r="Q51" s="24"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="24"/>
+      <c r="T51" s="5"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="24"/>
+      <c r="L52" s="24"/>
+      <c r="M52" s="24"/>
+      <c r="N52" s="24"/>
+      <c r="O52" s="24"/>
+      <c r="P52" s="24"/>
+      <c r="Q52" s="24"/>
+      <c r="R52" s="24"/>
+      <c r="S52" s="24"/>
+      <c r="T52" s="5"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="24"/>
+      <c r="L53" s="24"/>
+      <c r="M53" s="24"/>
+      <c r="N53" s="24"/>
+      <c r="O53" s="24"/>
+      <c r="P53" s="24"/>
+      <c r="Q53" s="24"/>
+      <c r="R53" s="24"/>
+      <c r="S53" s="24"/>
+      <c r="T53" s="5"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="24"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="24"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="24"/>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="24"/>
+      <c r="S54" s="24"/>
+      <c r="T54" s="5"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="24"/>
+      <c r="L55" s="24"/>
+      <c r="M55" s="24"/>
+      <c r="N55" s="24"/>
+      <c r="O55" s="24"/>
+      <c r="P55" s="24"/>
+      <c r="Q55" s="24"/>
+      <c r="R55" s="24"/>
+      <c r="S55" s="24"/>
+      <c r="T55" s="5"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="24"/>
+      <c r="L56" s="24"/>
+      <c r="M56" s="24"/>
+      <c r="N56" s="24"/>
+      <c r="O56" s="24"/>
+      <c r="P56" s="24"/>
+      <c r="Q56" s="24"/>
+      <c r="R56" s="24"/>
+      <c r="S56" s="24"/>
+      <c r="T56" s="5"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="24"/>
+      <c r="J57" s="24"/>
+      <c r="K57" s="24"/>
+      <c r="L57" s="24"/>
+      <c r="M57" s="24"/>
+      <c r="N57" s="24"/>
+      <c r="O57" s="24"/>
+      <c r="P57" s="24"/>
+      <c r="Q57" s="24"/>
+      <c r="R57" s="24"/>
+      <c r="S57" s="24"/>
+      <c r="T57" s="5"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
+      <c r="O58" s="24"/>
+      <c r="P58" s="24"/>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="24"/>
+      <c r="S58" s="24"/>
+      <c r="T58" s="5"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="24"/>
+      <c r="J59" s="24"/>
+      <c r="K59" s="24"/>
+      <c r="L59" s="24"/>
+      <c r="M59" s="24"/>
+      <c r="N59" s="24"/>
+      <c r="O59" s="24"/>
+      <c r="P59" s="24"/>
+      <c r="Q59" s="24"/>
+      <c r="R59" s="24"/>
+      <c r="S59" s="24"/>
+      <c r="T59" s="5"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="24"/>
+      <c r="J60" s="24"/>
+      <c r="K60" s="24"/>
+      <c r="L60" s="24"/>
+      <c r="M60" s="24"/>
+      <c r="N60" s="24"/>
+      <c r="O60" s="24"/>
+      <c r="P60" s="24"/>
+      <c r="Q60" s="24"/>
+      <c r="R60" s="24"/>
+      <c r="S60" s="24"/>
+      <c r="T60" s="5"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="24"/>
+      <c r="J61" s="24"/>
+      <c r="K61" s="24"/>
+      <c r="L61" s="24"/>
+      <c r="M61" s="24"/>
+      <c r="N61" s="24"/>
+      <c r="O61" s="24"/>
+      <c r="P61" s="24"/>
+      <c r="Q61" s="24"/>
+      <c r="R61" s="24"/>
+      <c r="S61" s="24"/>
+      <c r="T61" s="5"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="24"/>
+      <c r="J62" s="24"/>
+      <c r="K62" s="24"/>
+      <c r="L62" s="24"/>
+      <c r="M62" s="24"/>
+      <c r="N62" s="24"/>
+      <c r="O62" s="24"/>
+      <c r="P62" s="24"/>
+      <c r="Q62" s="24"/>
+      <c r="R62" s="24"/>
+      <c r="S62" s="24"/>
+      <c r="T62" s="5"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
+      <c r="K63" s="24"/>
+      <c r="L63" s="24"/>
+      <c r="M63" s="24"/>
+      <c r="N63" s="24"/>
+      <c r="O63" s="24"/>
+      <c r="P63" s="24"/>
+      <c r="Q63" s="24"/>
+      <c r="R63" s="24"/>
+      <c r="S63" s="24"/>
+      <c r="T63" s="5"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="24"/>
+      <c r="J64" s="24"/>
+      <c r="K64" s="24"/>
+      <c r="L64" s="24"/>
+      <c r="M64" s="24"/>
+      <c r="N64" s="24"/>
+      <c r="O64" s="24"/>
+      <c r="P64" s="24"/>
+      <c r="Q64" s="24"/>
+      <c r="R64" s="24"/>
+      <c r="S64" s="24"/>
+      <c r="T64" s="5"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="24"/>
+      <c r="J65" s="24"/>
+      <c r="K65" s="24"/>
+      <c r="L65" s="24"/>
+      <c r="M65" s="24"/>
+      <c r="N65" s="24"/>
+      <c r="O65" s="24"/>
+      <c r="P65" s="24"/>
+      <c r="Q65" s="24"/>
+      <c r="R65" s="24"/>
+      <c r="S65" s="24"/>
+      <c r="T65" s="5"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="24"/>
+      <c r="J66" s="24"/>
+      <c r="K66" s="24"/>
+      <c r="L66" s="24"/>
+      <c r="M66" s="24"/>
+      <c r="N66" s="24"/>
+      <c r="O66" s="24"/>
+      <c r="P66" s="24"/>
+      <c r="Q66" s="24"/>
+      <c r="R66" s="24"/>
+      <c r="S66" s="24"/>
+      <c r="T66" s="5"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="24"/>
+      <c r="J67" s="24"/>
+      <c r="K67" s="24"/>
+      <c r="L67" s="24"/>
+      <c r="M67" s="24"/>
+      <c r="N67" s="24"/>
+      <c r="O67" s="24"/>
+      <c r="P67" s="24"/>
+      <c r="Q67" s="24"/>
+      <c r="R67" s="24"/>
+      <c r="S67" s="24"/>
+      <c r="T67" s="5"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="24"/>
+      <c r="J68" s="24"/>
+      <c r="K68" s="24"/>
+      <c r="L68" s="24"/>
+      <c r="M68" s="24"/>
+      <c r="N68" s="24"/>
+      <c r="O68" s="24"/>
+      <c r="P68" s="24"/>
+      <c r="Q68" s="24"/>
+      <c r="R68" s="24"/>
+      <c r="S68" s="24"/>
+      <c r="T68" s="5"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="24"/>
+      <c r="J69" s="24"/>
+      <c r="K69" s="24"/>
+      <c r="L69" s="24"/>
+      <c r="M69" s="24"/>
+      <c r="N69" s="24"/>
+      <c r="O69" s="24"/>
+      <c r="P69" s="24"/>
+      <c r="Q69" s="24"/>
+      <c r="R69" s="24"/>
+      <c r="S69" s="24"/>
+      <c r="T69" s="5"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="24"/>
+      <c r="L70" s="24"/>
+      <c r="M70" s="24"/>
+      <c r="N70" s="24"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="24"/>
+      <c r="Q70" s="24"/>
+      <c r="R70" s="24"/>
+      <c r="S70" s="24"/>
+      <c r="T70" s="5"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
+      <c r="J71" s="24"/>
+      <c r="K71" s="24"/>
+      <c r="L71" s="24"/>
+      <c r="M71" s="24"/>
+      <c r="N71" s="24"/>
+      <c r="O71" s="24"/>
+      <c r="P71" s="24"/>
+      <c r="Q71" s="24"/>
+      <c r="R71" s="24"/>
+      <c r="S71" s="24"/>
+      <c r="T71" s="5"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="24"/>
+      <c r="K72" s="24"/>
+      <c r="L72" s="24"/>
+      <c r="M72" s="24"/>
+      <c r="N72" s="24"/>
+      <c r="O72" s="24"/>
+      <c r="P72" s="24"/>
+      <c r="Q72" s="24"/>
+      <c r="R72" s="24"/>
+      <c r="S72" s="24"/>
+      <c r="T72" s="5"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+      <c r="J73" s="24"/>
+      <c r="K73" s="24"/>
+      <c r="L73" s="24"/>
+      <c r="M73" s="24"/>
+      <c r="N73" s="24"/>
+      <c r="O73" s="24"/>
+      <c r="P73" s="24"/>
+      <c r="Q73" s="24"/>
+      <c r="R73" s="24"/>
+      <c r="S73" s="24"/>
+      <c r="T73" s="5"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="24"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="24"/>
+      <c r="L74" s="24"/>
+      <c r="M74" s="24"/>
+      <c r="N74" s="24"/>
+      <c r="O74" s="24"/>
+      <c r="P74" s="24"/>
+      <c r="Q74" s="24"/>
+      <c r="R74" s="24"/>
+      <c r="S74" s="24"/>
+      <c r="T74" s="5"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="24"/>
+      <c r="L75" s="24"/>
+      <c r="M75" s="24"/>
+      <c r="N75" s="24"/>
+      <c r="O75" s="24"/>
+      <c r="P75" s="24"/>
+      <c r="Q75" s="24"/>
+      <c r="R75" s="24"/>
+      <c r="S75" s="24"/>
+      <c r="T75" s="5"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="24"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="24"/>
+      <c r="L76" s="24"/>
+      <c r="M76" s="24"/>
+      <c r="N76" s="24"/>
+      <c r="O76" s="24"/>
+      <c r="P76" s="24"/>
+      <c r="Q76" s="24"/>
+      <c r="R76" s="24"/>
+      <c r="S76" s="24"/>
+      <c r="T76" s="5"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="24"/>
+      <c r="K77" s="24"/>
+      <c r="L77" s="24"/>
+      <c r="M77" s="24"/>
+      <c r="N77" s="24"/>
+      <c r="O77" s="24"/>
+      <c r="P77" s="24"/>
+      <c r="Q77" s="24"/>
+      <c r="R77" s="24"/>
+      <c r="S77" s="24"/>
+      <c r="T77" s="5"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="24"/>
+      <c r="L78" s="24"/>
+      <c r="M78" s="24"/>
+      <c r="N78" s="24"/>
+      <c r="O78" s="24"/>
+      <c r="P78" s="24"/>
+      <c r="Q78" s="24"/>
+      <c r="R78" s="24"/>
+      <c r="S78" s="24"/>
+      <c r="T78" s="5"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+      <c r="K79" s="24"/>
+      <c r="L79" s="24"/>
+      <c r="M79" s="24"/>
+      <c r="N79" s="24"/>
+      <c r="O79" s="24"/>
+      <c r="P79" s="24"/>
+      <c r="Q79" s="24"/>
+      <c r="R79" s="24"/>
+      <c r="S79" s="24"/>
+      <c r="T79" s="5"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="24"/>
+      <c r="L80" s="24"/>
+      <c r="M80" s="24"/>
+      <c r="N80" s="24"/>
+      <c r="O80" s="24"/>
+      <c r="P80" s="24"/>
+      <c r="Q80" s="24"/>
+      <c r="R80" s="24"/>
+      <c r="S80" s="24"/>
+      <c r="T80" s="5"/>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24"/>
+      <c r="K81" s="24"/>
+      <c r="L81" s="24"/>
+      <c r="M81" s="24"/>
+      <c r="N81" s="24"/>
+      <c r="O81" s="24"/>
+      <c r="P81" s="24"/>
+      <c r="Q81" s="24"/>
+      <c r="R81" s="24"/>
+      <c r="S81" s="24"/>
+      <c r="T81" s="5"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="24"/>
+      <c r="J82" s="24"/>
+      <c r="K82" s="24"/>
+      <c r="L82" s="24"/>
+      <c r="M82" s="24"/>
+      <c r="N82" s="24"/>
+      <c r="O82" s="24"/>
+      <c r="P82" s="24"/>
+      <c r="Q82" s="24"/>
+      <c r="R82" s="24"/>
+      <c r="S82" s="24"/>
+      <c r="T82" s="5"/>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24"/>
+      <c r="H83" s="24"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="24"/>
+      <c r="K83" s="24"/>
+      <c r="L83" s="24"/>
+      <c r="M83" s="24"/>
+      <c r="N83" s="24"/>
+      <c r="O83" s="24"/>
+      <c r="P83" s="24"/>
+      <c r="Q83" s="24"/>
+      <c r="R83" s="24"/>
+      <c r="S83" s="24"/>
+      <c r="T83" s="5"/>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="24"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="24"/>
+      <c r="N84" s="24"/>
+      <c r="O84" s="24"/>
+      <c r="P84" s="24"/>
+      <c r="Q84" s="24"/>
+      <c r="R84" s="24"/>
+      <c r="S84" s="24"/>
+      <c r="T84" s="5"/>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="24"/>
+      <c r="K85" s="24"/>
+      <c r="L85" s="24"/>
+      <c r="M85" s="24"/>
+      <c r="N85" s="24"/>
+      <c r="O85" s="24"/>
+      <c r="P85" s="24"/>
+      <c r="Q85" s="24"/>
+      <c r="R85" s="24"/>
+      <c r="S85" s="24"/>
+      <c r="T85" s="5"/>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="24"/>
+      <c r="L86" s="24"/>
+      <c r="M86" s="24"/>
+      <c r="N86" s="24"/>
+      <c r="O86" s="24"/>
+      <c r="P86" s="24"/>
+      <c r="Q86" s="24"/>
+      <c r="R86" s="24"/>
+      <c r="S86" s="24"/>
+      <c r="T86" s="5"/>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="24"/>
+      <c r="K87" s="24"/>
+      <c r="L87" s="24"/>
+      <c r="M87" s="24"/>
+      <c r="N87" s="24"/>
+      <c r="O87" s="24"/>
+      <c r="P87" s="24"/>
+      <c r="Q87" s="24"/>
+      <c r="R87" s="24"/>
+      <c r="S87" s="24"/>
+      <c r="T87" s="5"/>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="24"/>
+      <c r="L88" s="24"/>
+      <c r="M88" s="24"/>
+      <c r="N88" s="24"/>
+      <c r="O88" s="24"/>
+      <c r="P88" s="24"/>
+      <c r="Q88" s="24"/>
+      <c r="R88" s="24"/>
+      <c r="S88" s="24"/>
+      <c r="T88" s="5"/>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+      <c r="J89" s="24"/>
+      <c r="K89" s="24"/>
+      <c r="L89" s="24"/>
+      <c r="M89" s="24"/>
+      <c r="N89" s="24"/>
+      <c r="O89" s="24"/>
+      <c r="P89" s="24"/>
+      <c r="Q89" s="24"/>
+      <c r="R89" s="24"/>
+      <c r="S89" s="24"/>
+      <c r="T89" s="5"/>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="24"/>
+      <c r="L90" s="24"/>
+      <c r="M90" s="24"/>
+      <c r="N90" s="24"/>
+      <c r="O90" s="24"/>
+      <c r="P90" s="24"/>
+      <c r="Q90" s="24"/>
+      <c r="R90" s="24"/>
+      <c r="S90" s="24"/>
+      <c r="T90" s="5"/>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+      <c r="J91" s="24"/>
+      <c r="K91" s="24"/>
+      <c r="L91" s="24"/>
+      <c r="M91" s="24"/>
+      <c r="N91" s="24"/>
+      <c r="O91" s="24"/>
+      <c r="P91" s="24"/>
+      <c r="Q91" s="24"/>
+      <c r="R91" s="24"/>
+      <c r="S91" s="24"/>
+      <c r="T91" s="5"/>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+      <c r="J92" s="24"/>
+      <c r="K92" s="24"/>
+      <c r="L92" s="24"/>
+      <c r="M92" s="24"/>
+      <c r="N92" s="24"/>
+      <c r="O92" s="24"/>
+      <c r="P92" s="24"/>
+      <c r="Q92" s="24"/>
+      <c r="R92" s="24"/>
+      <c r="S92" s="24"/>
+      <c r="T92" s="5"/>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="24"/>
+      <c r="J93" s="24"/>
+      <c r="K93" s="24"/>
+      <c r="L93" s="24"/>
+      <c r="M93" s="24"/>
+      <c r="N93" s="24"/>
+      <c r="O93" s="24"/>
+      <c r="P93" s="24"/>
+      <c r="Q93" s="24"/>
+      <c r="R93" s="24"/>
+      <c r="S93" s="24"/>
+      <c r="T93" s="5"/>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="24"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="24"/>
+      <c r="J94" s="24"/>
+      <c r="K94" s="24"/>
+      <c r="L94" s="24"/>
+      <c r="M94" s="24"/>
+      <c r="N94" s="24"/>
+      <c r="O94" s="24"/>
+      <c r="P94" s="24"/>
+      <c r="Q94" s="24"/>
+      <c r="R94" s="24"/>
+      <c r="S94" s="24"/>
+      <c r="T94" s="5"/>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24"/>
+      <c r="J95" s="24"/>
+      <c r="K95" s="24"/>
+      <c r="L95" s="24"/>
+      <c r="M95" s="24"/>
+      <c r="N95" s="24"/>
+      <c r="O95" s="24"/>
+      <c r="P95" s="24"/>
+      <c r="Q95" s="24"/>
+      <c r="R95" s="24"/>
+      <c r="S95" s="24"/>
+      <c r="T95" s="5"/>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="24"/>
+      <c r="I96" s="24"/>
+      <c r="J96" s="24"/>
+      <c r="K96" s="24"/>
+      <c r="L96" s="24"/>
+      <c r="M96" s="24"/>
+      <c r="N96" s="24"/>
+      <c r="O96" s="24"/>
+      <c r="P96" s="24"/>
+      <c r="Q96" s="24"/>
+      <c r="R96" s="24"/>
+      <c r="S96" s="24"/>
+      <c r="T96" s="5"/>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
+      <c r="I97" s="24"/>
+      <c r="J97" s="24"/>
+      <c r="K97" s="24"/>
+      <c r="L97" s="24"/>
+      <c r="M97" s="24"/>
+      <c r="N97" s="24"/>
+      <c r="O97" s="24"/>
+      <c r="P97" s="24"/>
+      <c r="Q97" s="24"/>
+      <c r="R97" s="24"/>
+      <c r="S97" s="24"/>
+      <c r="T97" s="5"/>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
+      <c r="I98" s="24"/>
+      <c r="J98" s="24"/>
+      <c r="K98" s="24"/>
+      <c r="L98" s="24"/>
+      <c r="M98" s="24"/>
+      <c r="N98" s="24"/>
+      <c r="O98" s="24"/>
+      <c r="P98" s="24"/>
+      <c r="Q98" s="24"/>
+      <c r="R98" s="24"/>
+      <c r="S98" s="24"/>
+      <c r="T98" s="5"/>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24"/>
+      <c r="H99" s="24"/>
+      <c r="I99" s="24"/>
+      <c r="J99" s="24"/>
+      <c r="K99" s="24"/>
+      <c r="L99" s="24"/>
+      <c r="M99" s="24"/>
+      <c r="N99" s="24"/>
+      <c r="O99" s="24"/>
+      <c r="P99" s="24"/>
+      <c r="Q99" s="24"/>
+      <c r="R99" s="24"/>
+      <c r="S99" s="24"/>
+      <c r="T99" s="5"/>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+      <c r="I100" s="24"/>
+      <c r="J100" s="24"/>
+      <c r="K100" s="24"/>
+      <c r="L100" s="24"/>
+      <c r="M100" s="24"/>
+      <c r="N100" s="24"/>
+      <c r="O100" s="24"/>
+      <c r="P100" s="24"/>
+      <c r="Q100" s="24"/>
+      <c r="R100" s="24"/>
+      <c r="S100" s="24"/>
+      <c r="T100" s="5"/>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="24"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
+      <c r="I101" s="24"/>
+      <c r="J101" s="24"/>
+      <c r="K101" s="24"/>
+      <c r="L101" s="24"/>
+      <c r="M101" s="24"/>
+      <c r="N101" s="24"/>
+      <c r="O101" s="24"/>
+      <c r="P101" s="24"/>
+      <c r="Q101" s="24"/>
+      <c r="R101" s="24"/>
+      <c r="S101" s="24"/>
+      <c r="T101" s="5"/>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A102" s="4"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="24"/>
+      <c r="K102" s="24"/>
+      <c r="L102" s="24"/>
+      <c r="M102" s="24"/>
+      <c r="N102" s="24"/>
+      <c r="O102" s="24"/>
+      <c r="P102" s="24"/>
+      <c r="Q102" s="24"/>
+      <c r="R102" s="24"/>
+      <c r="S102" s="24"/>
+      <c r="T102" s="5"/>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A103" s="6"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="7"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="7"/>
+      <c r="P103" s="7"/>
+      <c r="Q103" s="7"/>
+      <c r="R103" s="7"/>
+      <c r="S103" s="7"/>
+      <c r="T103" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Set Datatype - Collections in Apex
</commit_message>
<xml_diff>
--- a/me/2.Apex-Fundamentals.xlsx
+++ b/me/2.Apex-Fundamentals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980E02BA-A6E9-44BE-9D4D-1DB394918296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CD1B98-A41A-49CD-A1DB-146229C39C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hello World" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Escape Character" sheetId="4" r:id="rId4"/>
     <sheet name="Adding Comments" sheetId="5" r:id="rId5"/>
     <sheet name="List Collections Datatype" sheetId="6" r:id="rId6"/>
+    <sheet name="Set Collections Datatype" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="140">
   <si>
     <t>Mở Developer Console trên tab mới</t>
   </si>
@@ -471,6 +472,72 @@
   </si>
   <si>
     <t>https://developer.salesforce.com/docs/atlas.en-us.apexref.meta/apexref/apex_methods_system_list.htm</t>
+  </si>
+  <si>
+    <t>List dùng để lưu các item có cùng kiểu dữ liệu</t>
+  </si>
+  <si>
+    <t>Set dùng để lưu các item có cùng kiểu dữ liệu</t>
+  </si>
+  <si>
+    <t>Thêm phần tử vào vị trí thứ 4, khi đó các</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item từ giá trị 89897764 sẽ được dịch </t>
+  </si>
+  <si>
+    <t>chuyển đến vị trí tiếp theo của vị trí cũ</t>
+  </si>
+  <si>
+    <t>Khác với List, Set lưu các item ko có thứ tự(Set ko dùng index nên nó được gọi là unordered)</t>
+  </si>
+  <si>
+    <t>Khác với List thì Set ko cho phép duplicate value</t>
+  </si>
+  <si>
+    <t>7.set-collection-datatype.txt</t>
+  </si>
+  <si>
+    <t>salesforce\2.Apex-Fundamentals\7.set-collection-datatype.txt</t>
+  </si>
+  <si>
+    <t>Set&lt;Integer&gt; rollNumbers = new Set&lt;Integer&gt;{11008890, 11008100, 11007231};</t>
+  </si>
+  <si>
+    <t>// adding duplicate values - NOT ALLOWED</t>
+  </si>
+  <si>
+    <t>// check if set has an item</t>
+  </si>
+  <si>
+    <t>System.debug(rollNumbers.contains(89897764));</t>
+  </si>
+  <si>
+    <t>System.debug(rollNumbers.contains(345345));</t>
+  </si>
+  <si>
+    <t>// delete an item</t>
+  </si>
+  <si>
+    <t>rollNumbers.remove(89897765);</t>
+  </si>
+  <si>
+    <t>// get set size</t>
+  </si>
+  <si>
+    <t>// check if set is empty</t>
+  </si>
+  <si>
+    <t>System.debug(rollNumbers.isEmpty());</t>
+  </si>
+  <si>
+    <t>// remove all items</t>
+  </si>
+  <si>
+    <t>Giá trị 89897767 đã tồn tại nên sẽ ko được thêm vào</t>
+  </si>
+  <si>
+    <t>Xóa 1 item nên còn 5 item</t>
   </si>
 </sst>
 </file>
@@ -620,10 +687,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2550,13 +2617,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>193860</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>94130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>468679</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>122059</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2594,13 +2661,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>168087</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>56030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>510986</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>48555</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2638,13 +2705,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>549088</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>493059</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2691,13 +2758,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>56031</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>89648</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>313766</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2729,6 +2796,320 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE434A00-D99C-51EB-5077-3A2AEE520C67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="13054853"/>
+          <a:ext cx="10892118" cy="1792941"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17B76D88-5F9F-1ADE-9604-79B5B5038C9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7507941" y="13290176"/>
+          <a:ext cx="6432177" cy="1535206"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>303174</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>132644</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAE9F204-56C8-EA44-D24C-EBE2DCCDA558}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9239250" y="3819525"/>
+          <a:ext cx="13009524" cy="5647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48460A3C-461B-2D32-C1CD-0E4F13CD89DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1809750" y="4543425"/>
+          <a:ext cx="9525" cy="1228725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E448705C-734B-60FA-7DD1-8DF70D3CBC4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7315200" y="6819900"/>
+          <a:ext cx="3962400" cy="1228725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{675D99D0-0578-F9A1-7E1A-935C70B1DCBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="7381875"/>
+          <a:ext cx="809625" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5321,7 +5702,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>116</v>
       </c>
       <c r="C3" s="2"/>
@@ -5345,632 +5726,122 @@
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
       <c r="T4" s="5"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
       <c r="T5" s="5"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
       <c r="T8" s="5"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
       <c r="T10" s="5"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
       <c r="T11" s="5"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
       <c r="T12" s="5"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
       <c r="T13" s="5"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
       <c r="T14" s="5"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
       <c r="T15" s="5"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
       <c r="T17" s="5"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
       <c r="T18" s="5"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
       <c r="T19" s="5"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
       <c r="T20" s="5"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
       <c r="T22" s="5"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
       <c r="T24" s="5"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
       <c r="T25" s="5"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
       <c r="T26" s="5"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
       <c r="T27" s="5"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
       <c r="T28" s="5"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
       <c r="T29" s="5"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
       <c r="T31" s="5"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
       <c r="T32" s="5"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
       <c r="T33" s="5"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -7433,1688 +7304,1000 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC5A17F-325A-41A3-9954-AF1931AC7357}">
-  <dimension ref="A2:AG95"/>
+  <dimension ref="A2:AG96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="O38" s="1"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
-      <c r="X38" s="2"/>
-      <c r="Y38" s="2"/>
-      <c r="Z38" s="2"/>
-      <c r="AA38" s="2"/>
-      <c r="AB38" s="2"/>
-      <c r="AC38" s="2"/>
-      <c r="AD38" s="2"/>
-      <c r="AE38" s="2"/>
-      <c r="AF38" s="2"/>
-      <c r="AG38" s="3"/>
-    </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="O39" s="4"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
-      <c r="U39" s="15"/>
-      <c r="V39" s="15"/>
-      <c r="W39" s="15"/>
-      <c r="X39" s="15"/>
-      <c r="Y39" s="15"/>
-      <c r="Z39" s="15"/>
-      <c r="AA39" s="15"/>
-      <c r="AB39" s="15"/>
-      <c r="AC39" s="15"/>
-      <c r="AD39" s="15"/>
-      <c r="AE39" s="15"/>
-      <c r="AF39" s="15"/>
-      <c r="AG39" s="5"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="3"/>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="O40" s="4"/>
+      <c r="AG40" s="5"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O40" s="4"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
-      <c r="U40" s="15"/>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-      <c r="X40" s="15"/>
-      <c r="Y40" s="15"/>
-      <c r="Z40" s="15"/>
-      <c r="AA40" s="15"/>
-      <c r="AB40" s="15"/>
-      <c r="AC40" s="15"/>
-      <c r="AD40" s="15"/>
-      <c r="AE40" s="15"/>
-      <c r="AF40" s="15"/>
-      <c r="AG40" s="5"/>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+      <c r="O41" s="4"/>
+      <c r="AG41" s="5"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
-      <c r="U41" s="15"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="15"/>
-      <c r="X41" s="15"/>
-      <c r="Y41" s="15"/>
-      <c r="Z41" s="15"/>
-      <c r="AA41" s="15"/>
-      <c r="AB41" s="15"/>
-      <c r="AC41" s="15"/>
-      <c r="AD41" s="15"/>
-      <c r="AE41" s="15"/>
-      <c r="AF41" s="15"/>
-      <c r="AG41" s="5"/>
-    </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
-      <c r="C42" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="5"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="3"/>
       <c r="O42" s="4"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
-      <c r="U42" s="15"/>
-      <c r="V42" s="15"/>
-      <c r="W42" s="15"/>
-      <c r="X42" s="15"/>
-      <c r="Y42" s="15"/>
-      <c r="Z42" s="15"/>
-      <c r="AA42" s="15"/>
-      <c r="AB42" s="15"/>
-      <c r="AC42" s="15"/>
-      <c r="AD42" s="15"/>
-      <c r="AE42" s="15"/>
-      <c r="AF42" s="15"/>
       <c r="AG42" s="5"/>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
-      <c r="D43" t="s">
-        <v>12</v>
+      <c r="C43" t="s">
+        <v>11</v>
       </c>
       <c r="F43" s="5"/>
       <c r="O43" s="4"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="15"/>
-      <c r="AA43" s="15"/>
-      <c r="AB43" s="15"/>
-      <c r="AC43" s="15"/>
-      <c r="AD43" s="15"/>
-      <c r="AE43" s="15"/>
-      <c r="AF43" s="15"/>
       <c r="AG43" s="5"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F44" s="5"/>
       <c r="O44" s="4"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-      <c r="AA44" s="15"/>
-      <c r="AB44" s="15"/>
-      <c r="AC44" s="15"/>
-      <c r="AD44" s="15"/>
-      <c r="AE44" s="15"/>
-      <c r="AF44" s="15"/>
       <c r="AG44" s="5"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="F45" s="5"/>
       <c r="O45" s="4"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
-      <c r="T45" s="15"/>
-      <c r="U45" s="15"/>
-      <c r="V45" s="15"/>
-      <c r="W45" s="15"/>
-      <c r="X45" s="15"/>
-      <c r="Y45" s="15"/>
-      <c r="Z45" s="15"/>
-      <c r="AA45" s="15"/>
-      <c r="AB45" s="15"/>
-      <c r="AC45" s="15"/>
-      <c r="AD45" s="15"/>
-      <c r="AE45" s="15"/>
-      <c r="AF45" s="15"/>
       <c r="AG45" s="5"/>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="F46" s="5"/>
       <c r="O46" s="4"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="15"/>
-      <c r="T46" s="15"/>
-      <c r="U46" s="15"/>
-      <c r="V46" s="15"/>
-      <c r="W46" s="15"/>
-      <c r="X46" s="15"/>
-      <c r="Y46" s="15"/>
-      <c r="Z46" s="15"/>
-      <c r="AA46" s="15"/>
-      <c r="AB46" s="15"/>
-      <c r="AC46" s="15"/>
-      <c r="AD46" s="15"/>
-      <c r="AE46" s="15"/>
-      <c r="AF46" s="15"/>
       <c r="AG46" s="5"/>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="D47" s="14" t="s">
-        <v>81</v>
+      <c r="D47" t="s">
+        <v>77</v>
       </c>
       <c r="F47" s="5"/>
       <c r="O47" s="4"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
-      <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
-      <c r="V47" s="15"/>
-      <c r="W47" s="15"/>
-      <c r="X47" s="15"/>
-      <c r="Y47" s="15"/>
-      <c r="Z47" s="15"/>
-      <c r="AA47" s="15"/>
-      <c r="AB47" s="15"/>
-      <c r="AC47" s="15"/>
-      <c r="AD47" s="15"/>
-      <c r="AE47" s="15"/>
-      <c r="AF47" s="15"/>
       <c r="AG47" s="5"/>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
-      <c r="D48" s="10" t="s">
+      <c r="D48" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="O48" s="4"/>
+      <c r="AG48" s="5"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="D49" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F48" s="5"/>
-      <c r="G48" t="s">
+      <c r="F49" s="5"/>
+      <c r="G49" t="s">
         <v>17</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H49" t="s">
         <v>16</v>
       </c>
-      <c r="O48" s="4"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="15"/>
-      <c r="U48" s="15"/>
-      <c r="V48" s="15"/>
-      <c r="W48" s="15"/>
-      <c r="X48" s="15"/>
-      <c r="Y48" s="15"/>
-      <c r="Z48" s="15"/>
-      <c r="AA48" s="15"/>
-      <c r="AB48" s="15"/>
-      <c r="AC48" s="15"/>
-      <c r="AD48" s="15"/>
-      <c r="AE48" s="15"/>
-      <c r="AF48" s="15"/>
-      <c r="AG48" s="5"/>
-    </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
       <c r="O49" s="4"/>
-      <c r="P49" s="15"/>
-      <c r="Q49" s="15"/>
-      <c r="R49" s="15"/>
-      <c r="S49" s="15"/>
-      <c r="T49" s="15"/>
-      <c r="U49" s="15"/>
-      <c r="V49" s="15"/>
-      <c r="W49" s="15"/>
-      <c r="X49" s="15"/>
-      <c r="Y49" s="15"/>
-      <c r="Z49" s="15"/>
-      <c r="AA49" s="15"/>
-      <c r="AB49" s="15"/>
-      <c r="AC49" s="15"/>
-      <c r="AD49" s="15"/>
-      <c r="AE49" s="15"/>
-      <c r="AF49" s="15"/>
       <c r="AG49" s="5"/>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
       <c r="O50" s="4"/>
-      <c r="P50" s="15"/>
-      <c r="Q50" s="15"/>
-      <c r="R50" s="15"/>
-      <c r="S50" s="15"/>
-      <c r="T50" s="15"/>
-      <c r="U50" s="15"/>
-      <c r="V50" s="15"/>
-      <c r="W50" s="15"/>
-      <c r="X50" s="15"/>
-      <c r="Y50" s="15"/>
-      <c r="Z50" s="15"/>
-      <c r="AA50" s="15"/>
-      <c r="AB50" s="15"/>
-      <c r="AC50" s="15"/>
-      <c r="AD50" s="15"/>
-      <c r="AE50" s="15"/>
-      <c r="AF50" s="15"/>
       <c r="AG50" s="5"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="O51" s="4"/>
-      <c r="P51" s="15"/>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="15"/>
-      <c r="S51" s="15"/>
-      <c r="T51" s="15"/>
-      <c r="U51" s="15"/>
-      <c r="V51" s="15"/>
-      <c r="W51" s="15"/>
-      <c r="X51" s="15"/>
-      <c r="Y51" s="15"/>
-      <c r="Z51" s="15"/>
-      <c r="AA51" s="15"/>
-      <c r="AB51" s="15"/>
-      <c r="AC51" s="15"/>
-      <c r="AD51" s="15"/>
-      <c r="AE51" s="15"/>
-      <c r="AF51" s="15"/>
       <c r="AG51" s="5"/>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="O52" s="4"/>
+      <c r="AG52" s="5"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>91</v>
       </c>
-      <c r="O52" s="4"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="15"/>
-      <c r="R52" s="15"/>
-      <c r="S52" s="15"/>
-      <c r="T52" s="15"/>
-      <c r="U52" s="15"/>
-      <c r="V52" s="15"/>
-      <c r="W52" s="15"/>
-      <c r="X52" s="15"/>
-      <c r="Y52" s="15"/>
-      <c r="Z52" s="15"/>
-      <c r="AA52" s="15"/>
-      <c r="AB52" s="15"/>
-      <c r="AC52" s="15"/>
-      <c r="AD52" s="15"/>
-      <c r="AE52" s="15"/>
-      <c r="AF52" s="15"/>
-      <c r="AG52" s="5"/>
-    </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
+      <c r="O53" s="4"/>
+      <c r="AG53" s="5"/>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="3"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="15"/>
-      <c r="T53" s="15"/>
-      <c r="U53" s="15"/>
-      <c r="V53" s="15"/>
-      <c r="W53" s="15"/>
-      <c r="X53" s="15"/>
-      <c r="Y53" s="15"/>
-      <c r="Z53" s="15"/>
-      <c r="AA53" s="15"/>
-      <c r="AB53" s="15"/>
-      <c r="AC53" s="15"/>
-      <c r="AD53" s="15"/>
-      <c r="AE53" s="15"/>
-      <c r="AF53" s="15"/>
-      <c r="AG53" s="5"/>
-    </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="3"/>
+      <c r="O54" s="4"/>
+      <c r="AG54" s="5"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="5"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="15"/>
-      <c r="T54" s="15"/>
-      <c r="U54" s="15"/>
-      <c r="V54" s="15"/>
-      <c r="W54" s="15"/>
-      <c r="X54" s="15"/>
-      <c r="Y54" s="15"/>
-      <c r="Z54" s="15"/>
-      <c r="AA54" s="15"/>
-      <c r="AB54" s="15"/>
-      <c r="AC54" s="15"/>
-      <c r="AD54" s="15"/>
-      <c r="AE54" s="15"/>
-      <c r="AF54" s="15"/>
-      <c r="AG54" s="5"/>
-    </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
       <c r="I55" s="5"/>
       <c r="O55" s="4"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
-      <c r="R55" s="15"/>
-      <c r="S55" s="15"/>
-      <c r="T55" s="15"/>
-      <c r="U55" s="15"/>
-      <c r="V55" s="15"/>
-      <c r="W55" s="15"/>
-      <c r="X55" s="15"/>
-      <c r="Y55" s="15"/>
-      <c r="Z55" s="15"/>
-      <c r="AA55" s="15"/>
-      <c r="AB55" s="15"/>
-      <c r="AC55" s="15"/>
-      <c r="AD55" s="15"/>
-      <c r="AE55" s="15"/>
-      <c r="AF55" s="15"/>
       <c r="AG55" s="5"/>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
+      <c r="B56" s="4"/>
       <c r="I56" s="5"/>
-      <c r="J56" t="s">
-        <v>17</v>
-      </c>
-      <c r="K56" t="s">
-        <v>113</v>
-      </c>
       <c r="O56" s="4"/>
-      <c r="P56" s="15"/>
-      <c r="Q56" s="15"/>
-      <c r="R56" s="15"/>
-      <c r="S56" s="15"/>
-      <c r="T56" s="15"/>
-      <c r="U56" s="15"/>
-      <c r="V56" s="15"/>
-      <c r="W56" s="15"/>
-      <c r="X56" s="15"/>
-      <c r="Y56" s="15"/>
-      <c r="Z56" s="15"/>
-      <c r="AA56" s="15"/>
-      <c r="AB56" s="15"/>
-      <c r="AC56" s="15"/>
-      <c r="AD56" s="15"/>
-      <c r="AE56" s="15"/>
-      <c r="AF56" s="15"/>
       <c r="AG56" s="5"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
+        <v>95</v>
+      </c>
       <c r="I57" s="5"/>
+      <c r="J57" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" t="s">
+        <v>113</v>
+      </c>
       <c r="O57" s="4"/>
-      <c r="P57" s="15"/>
-      <c r="Q57" s="15"/>
-      <c r="R57" s="15"/>
-      <c r="S57" s="15"/>
-      <c r="T57" s="15"/>
-      <c r="U57" s="15"/>
-      <c r="V57" s="15"/>
-      <c r="W57" s="15"/>
-      <c r="X57" s="15"/>
-      <c r="Y57" s="15"/>
-      <c r="Z57" s="15"/>
-      <c r="AA57" s="15"/>
-      <c r="AB57" s="15"/>
-      <c r="AC57" s="15"/>
-      <c r="AD57" s="15"/>
-      <c r="AE57" s="15"/>
-      <c r="AF57" s="15"/>
       <c r="AG57" s="5"/>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
+        <v>96</v>
+      </c>
       <c r="I58" s="5"/>
       <c r="O58" s="4"/>
-      <c r="P58" s="15"/>
-      <c r="Q58" s="15"/>
-      <c r="R58" s="15"/>
-      <c r="S58" s="15"/>
-      <c r="T58" s="15"/>
-      <c r="U58" s="15"/>
-      <c r="V58" s="15"/>
-      <c r="W58" s="15"/>
-      <c r="X58" s="15"/>
-      <c r="Y58" s="15"/>
-      <c r="Z58" s="15"/>
-      <c r="AA58" s="15"/>
-      <c r="AB58" s="15"/>
-      <c r="AC58" s="15"/>
-      <c r="AD58" s="15"/>
-      <c r="AE58" s="15"/>
-      <c r="AF58" s="15"/>
       <c r="AG58" s="5"/>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
+      <c r="B59" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="I59" s="5"/>
       <c r="O59" s="4"/>
-      <c r="P59" s="15"/>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="15"/>
-      <c r="S59" s="15"/>
-      <c r="T59" s="15"/>
-      <c r="U59" s="15"/>
-      <c r="V59" s="15"/>
-      <c r="W59" s="15"/>
-      <c r="X59" s="15"/>
-      <c r="Y59" s="15"/>
-      <c r="Z59" s="15"/>
-      <c r="AA59" s="15"/>
-      <c r="AB59" s="15"/>
-      <c r="AC59" s="15"/>
-      <c r="AD59" s="15"/>
-      <c r="AE59" s="15"/>
-      <c r="AF59" s="15"/>
       <c r="AG59" s="5"/>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
+      <c r="B60" s="4"/>
       <c r="I60" s="5"/>
       <c r="O60" s="4"/>
-      <c r="P60" s="15"/>
-      <c r="Q60" s="15"/>
-      <c r="R60" s="15"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="15"/>
-      <c r="U60" s="15"/>
-      <c r="V60" s="15"/>
-      <c r="W60" s="15"/>
-      <c r="X60" s="15"/>
-      <c r="Y60" s="15"/>
-      <c r="Z60" s="15"/>
-      <c r="AA60" s="15"/>
-      <c r="AB60" s="15"/>
-      <c r="AC60" s="15"/>
-      <c r="AD60" s="15"/>
-      <c r="AE60" s="15"/>
-      <c r="AF60" s="15"/>
       <c r="AG60" s="5"/>
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="15"/>
+      <c r="B61" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I61" s="5"/>
       <c r="O61" s="4"/>
-      <c r="P61" s="15"/>
-      <c r="Q61" s="15"/>
-      <c r="R61" s="15"/>
-      <c r="S61" s="15"/>
-      <c r="T61" s="15"/>
-      <c r="U61" s="15"/>
-      <c r="V61" s="15"/>
-      <c r="W61" s="15"/>
-      <c r="X61" s="15"/>
-      <c r="Y61" s="15"/>
-      <c r="Z61" s="15"/>
-      <c r="AA61" s="15"/>
-      <c r="AB61" s="15"/>
-      <c r="AC61" s="15"/>
-      <c r="AD61" s="15"/>
-      <c r="AE61" s="15"/>
-      <c r="AF61" s="15"/>
       <c r="AG61" s="5"/>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15"/>
+      <c r="B62" s="4"/>
       <c r="I62" s="5"/>
       <c r="O62" s="4"/>
-      <c r="P62" s="15"/>
-      <c r="Q62" s="15"/>
-      <c r="R62" s="15"/>
-      <c r="S62" s="15"/>
-      <c r="T62" s="15"/>
-      <c r="U62" s="15"/>
-      <c r="V62" s="15"/>
-      <c r="W62" s="15"/>
-      <c r="X62" s="15"/>
-      <c r="Y62" s="15"/>
-      <c r="Z62" s="15"/>
-      <c r="AA62" s="15"/>
-      <c r="AB62" s="15"/>
-      <c r="AC62" s="15"/>
-      <c r="AD62" s="15"/>
-      <c r="AE62" s="15"/>
-      <c r="AF62" s="15"/>
       <c r="AG62" s="5"/>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
+        <v>98</v>
+      </c>
       <c r="I63" s="5"/>
       <c r="O63" s="4"/>
-      <c r="P63" s="15"/>
-      <c r="Q63" s="15"/>
-      <c r="R63" s="15"/>
-      <c r="S63" s="15"/>
-      <c r="T63" s="15"/>
-      <c r="U63" s="15"/>
-      <c r="V63" s="15"/>
-      <c r="W63" s="15"/>
-      <c r="X63" s="15"/>
-      <c r="Y63" s="15"/>
-      <c r="Z63" s="15"/>
-      <c r="AA63" s="15"/>
-      <c r="AB63" s="15"/>
-      <c r="AC63" s="15"/>
-      <c r="AD63" s="15"/>
-      <c r="AE63" s="15"/>
-      <c r="AF63" s="15"/>
       <c r="AG63" s="5"/>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15"/>
+        <v>99</v>
+      </c>
       <c r="I64" s="5"/>
       <c r="O64" s="4"/>
-      <c r="P64" s="15"/>
-      <c r="Q64" s="15"/>
-      <c r="R64" s="15"/>
-      <c r="S64" s="15"/>
-      <c r="T64" s="15"/>
-      <c r="U64" s="15"/>
-      <c r="V64" s="15"/>
-      <c r="W64" s="15"/>
-      <c r="X64" s="15"/>
-      <c r="Y64" s="15"/>
-      <c r="Z64" s="15"/>
-      <c r="AA64" s="15"/>
-      <c r="AB64" s="15"/>
-      <c r="AC64" s="15"/>
-      <c r="AD64" s="15"/>
-      <c r="AE64" s="15"/>
-      <c r="AF64" s="15"/>
       <c r="AG64" s="5"/>
     </row>
     <row r="65" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
+        <v>100</v>
+      </c>
       <c r="I65" s="5"/>
       <c r="O65" s="4"/>
-      <c r="P65" s="15"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="15"/>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="15"/>
-      <c r="Z65" s="15"/>
-      <c r="AA65" s="15"/>
-      <c r="AB65" s="15"/>
-      <c r="AC65" s="15"/>
-      <c r="AD65" s="15"/>
-      <c r="AE65" s="15"/>
-      <c r="AF65" s="15"/>
       <c r="AG65" s="5"/>
     </row>
     <row r="66" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
+      <c r="B66" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="I66" s="5"/>
       <c r="O66" s="4"/>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="15"/>
-      <c r="R66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="15"/>
-      <c r="U66" s="15"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="15"/>
-      <c r="X66" s="15"/>
-      <c r="Y66" s="15"/>
-      <c r="Z66" s="15"/>
-      <c r="AA66" s="15"/>
-      <c r="AB66" s="15"/>
-      <c r="AC66" s="15"/>
-      <c r="AD66" s="15"/>
-      <c r="AE66" s="15"/>
-      <c r="AF66" s="15"/>
       <c r="AG66" s="5"/>
     </row>
     <row r="67" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
+      <c r="B67" s="4"/>
       <c r="I67" s="5"/>
       <c r="O67" s="4"/>
-      <c r="P67" s="15"/>
-      <c r="Q67" s="15"/>
-      <c r="R67" s="15"/>
-      <c r="S67" s="15"/>
-      <c r="T67" s="15"/>
-      <c r="U67" s="15"/>
-      <c r="V67" s="15"/>
-      <c r="W67" s="15"/>
-      <c r="X67" s="15"/>
-      <c r="Y67" s="15"/>
-      <c r="Z67" s="15"/>
-      <c r="AA67" s="15"/>
-      <c r="AB67" s="15"/>
-      <c r="AC67" s="15"/>
-      <c r="AD67" s="15"/>
-      <c r="AE67" s="15"/>
-      <c r="AF67" s="15"/>
       <c r="AG67" s="5"/>
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15"/>
+        <v>102</v>
+      </c>
       <c r="I68" s="5"/>
       <c r="O68" s="4"/>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="15"/>
-      <c r="U68" s="15"/>
-      <c r="V68" s="15"/>
-      <c r="W68" s="15"/>
-      <c r="X68" s="15"/>
-      <c r="Y68" s="15"/>
-      <c r="Z68" s="15"/>
-      <c r="AA68" s="15"/>
-      <c r="AB68" s="15"/>
-      <c r="AC68" s="15"/>
-      <c r="AD68" s="15"/>
-      <c r="AE68" s="15"/>
-      <c r="AF68" s="15"/>
       <c r="AG68" s="5"/>
     </row>
     <row r="69" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I69" s="5"/>
+      <c r="J69" t="s">
+        <v>17</v>
+      </c>
+      <c r="K69" t="s">
+        <v>120</v>
+      </c>
+      <c r="O69" s="4"/>
+      <c r="AG69" s="5"/>
+    </row>
+    <row r="70" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="5"/>
-      <c r="O69" s="4"/>
-      <c r="P69" s="15"/>
-      <c r="Q69" s="15"/>
-      <c r="R69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="15"/>
-      <c r="U69" s="15"/>
-      <c r="V69" s="15"/>
-      <c r="W69" s="15"/>
-      <c r="X69" s="15"/>
-      <c r="Y69" s="15"/>
-      <c r="Z69" s="15"/>
-      <c r="AA69" s="15"/>
-      <c r="AB69" s="15"/>
-      <c r="AC69" s="15"/>
-      <c r="AD69" s="15"/>
-      <c r="AE69" s="15"/>
-      <c r="AF69" s="15"/>
-      <c r="AG69" s="5"/>
-    </row>
-    <row r="70" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
       <c r="I70" s="5"/>
+      <c r="K70" t="s">
+        <v>121</v>
+      </c>
       <c r="O70" s="4"/>
-      <c r="P70" s="15"/>
-      <c r="Q70" s="15"/>
-      <c r="R70" s="15"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="15"/>
-      <c r="U70" s="15"/>
-      <c r="V70" s="15"/>
-      <c r="W70" s="15"/>
-      <c r="X70" s="15"/>
-      <c r="Y70" s="15"/>
-      <c r="Z70" s="15"/>
-      <c r="AA70" s="15"/>
-      <c r="AB70" s="15"/>
-      <c r="AC70" s="15"/>
-      <c r="AD70" s="15"/>
-      <c r="AE70" s="15"/>
-      <c r="AF70" s="15"/>
       <c r="AG70" s="5"/>
     </row>
     <row r="71" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
-      <c r="G71" s="15"/>
-      <c r="H71" s="15"/>
+      <c r="B71" s="4"/>
       <c r="I71" s="5"/>
+      <c r="K71" t="s">
+        <v>122</v>
+      </c>
       <c r="O71" s="4"/>
-      <c r="P71" s="15"/>
-      <c r="Q71" s="15"/>
-      <c r="R71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="15"/>
-      <c r="U71" s="15"/>
-      <c r="V71" s="15"/>
-      <c r="W71" s="15"/>
-      <c r="X71" s="15"/>
-      <c r="Y71" s="15"/>
-      <c r="Z71" s="15"/>
-      <c r="AA71" s="15"/>
-      <c r="AB71" s="15"/>
-      <c r="AC71" s="15"/>
-      <c r="AD71" s="15"/>
-      <c r="AE71" s="15"/>
-      <c r="AF71" s="15"/>
       <c r="AG71" s="5"/>
     </row>
     <row r="72" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
+        <v>104</v>
+      </c>
       <c r="I72" s="5"/>
       <c r="O72" s="4"/>
-      <c r="P72" s="15"/>
-      <c r="Q72" s="15"/>
-      <c r="R72" s="15"/>
-      <c r="S72" s="15"/>
-      <c r="T72" s="15"/>
-      <c r="U72" s="15"/>
-      <c r="V72" s="15"/>
-      <c r="W72" s="15"/>
-      <c r="X72" s="15"/>
-      <c r="Y72" s="15"/>
-      <c r="Z72" s="15"/>
-      <c r="AA72" s="15"/>
-      <c r="AB72" s="15"/>
-      <c r="AC72" s="15"/>
-      <c r="AD72" s="15"/>
-      <c r="AE72" s="15"/>
-      <c r="AF72" s="15"/>
       <c r="AG72" s="5"/>
     </row>
     <row r="73" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="15"/>
-      <c r="H73" s="15"/>
+      <c r="B73" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="I73" s="5"/>
       <c r="O73" s="4"/>
-      <c r="P73" s="15"/>
-      <c r="Q73" s="15"/>
-      <c r="R73" s="15"/>
-      <c r="S73" s="15"/>
-      <c r="T73" s="15"/>
-      <c r="U73" s="15"/>
-      <c r="V73" s="15"/>
-      <c r="W73" s="15"/>
-      <c r="X73" s="15"/>
-      <c r="Y73" s="15"/>
-      <c r="Z73" s="15"/>
-      <c r="AA73" s="15"/>
-      <c r="AB73" s="15"/>
-      <c r="AC73" s="15"/>
-      <c r="AD73" s="15"/>
-      <c r="AE73" s="15"/>
-      <c r="AF73" s="15"/>
       <c r="AG73" s="5"/>
     </row>
     <row r="74" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="15"/>
-      <c r="H74" s="15"/>
+      <c r="B74" s="4"/>
       <c r="I74" s="5"/>
       <c r="O74" s="4"/>
-      <c r="P74" s="15"/>
-      <c r="Q74" s="15"/>
-      <c r="R74" s="15"/>
-      <c r="S74" s="15"/>
-      <c r="T74" s="15"/>
-      <c r="U74" s="15"/>
-      <c r="V74" s="15"/>
-      <c r="W74" s="15"/>
-      <c r="X74" s="15"/>
-      <c r="Y74" s="15"/>
-      <c r="Z74" s="15"/>
-      <c r="AA74" s="15"/>
-      <c r="AB74" s="15"/>
-      <c r="AC74" s="15"/>
-      <c r="AD74" s="15"/>
-      <c r="AE74" s="15"/>
-      <c r="AF74" s="15"/>
       <c r="AG74" s="5"/>
     </row>
     <row r="75" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
-      <c r="H75" s="15"/>
+        <v>106</v>
+      </c>
       <c r="I75" s="5"/>
       <c r="O75" s="4"/>
-      <c r="P75" s="15"/>
-      <c r="Q75" s="15"/>
-      <c r="R75" s="15"/>
-      <c r="S75" s="15"/>
-      <c r="T75" s="15"/>
-      <c r="U75" s="15"/>
-      <c r="V75" s="15"/>
-      <c r="W75" s="15"/>
-      <c r="X75" s="15"/>
-      <c r="Y75" s="15"/>
-      <c r="Z75" s="15"/>
-      <c r="AA75" s="15"/>
-      <c r="AB75" s="15"/>
-      <c r="AC75" s="15"/>
-      <c r="AD75" s="15"/>
-      <c r="AE75" s="15"/>
-      <c r="AF75" s="15"/>
       <c r="AG75" s="5"/>
     </row>
     <row r="76" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="15"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
-      <c r="H76" s="15"/>
+        <v>107</v>
+      </c>
       <c r="I76" s="5"/>
       <c r="O76" s="4"/>
-      <c r="P76" s="15"/>
-      <c r="Q76" s="15"/>
-      <c r="R76" s="15"/>
-      <c r="S76" s="15"/>
-      <c r="T76" s="15"/>
-      <c r="U76" s="15"/>
-      <c r="V76" s="15"/>
-      <c r="W76" s="15"/>
-      <c r="X76" s="15"/>
-      <c r="Y76" s="15"/>
-      <c r="Z76" s="15"/>
-      <c r="AA76" s="15"/>
-      <c r="AB76" s="15"/>
-      <c r="AC76" s="15"/>
-      <c r="AD76" s="15"/>
-      <c r="AE76" s="15"/>
-      <c r="AF76" s="15"/>
       <c r="AG76" s="5"/>
     </row>
     <row r="77" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="15"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
+        <v>94</v>
+      </c>
       <c r="I77" s="5"/>
       <c r="O77" s="4"/>
-      <c r="P77" s="15"/>
-      <c r="Q77" s="15"/>
-      <c r="R77" s="15"/>
-      <c r="S77" s="15"/>
-      <c r="T77" s="15"/>
-      <c r="U77" s="15"/>
-      <c r="V77" s="15"/>
-      <c r="W77" s="15"/>
-      <c r="X77" s="15"/>
-      <c r="Y77" s="15"/>
-      <c r="Z77" s="15"/>
-      <c r="AA77" s="15"/>
-      <c r="AB77" s="15"/>
-      <c r="AC77" s="15"/>
-      <c r="AD77" s="15"/>
-      <c r="AE77" s="15"/>
-      <c r="AF77" s="15"/>
       <c r="AG77" s="5"/>
     </row>
     <row r="78" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
-      <c r="H78" s="15"/>
+      <c r="B78" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="I78" s="5"/>
       <c r="O78" s="4"/>
-      <c r="P78" s="15"/>
-      <c r="Q78" s="15"/>
-      <c r="R78" s="15"/>
-      <c r="S78" s="15"/>
-      <c r="T78" s="15"/>
-      <c r="U78" s="15"/>
-      <c r="V78" s="15"/>
-      <c r="W78" s="15"/>
-      <c r="X78" s="15"/>
-      <c r="Y78" s="15"/>
-      <c r="Z78" s="15"/>
-      <c r="AA78" s="15"/>
-      <c r="AB78" s="15"/>
-      <c r="AC78" s="15"/>
-      <c r="AD78" s="15"/>
-      <c r="AE78" s="15"/>
-      <c r="AF78" s="15"/>
       <c r="AG78" s="5"/>
     </row>
     <row r="79" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
+      <c r="B79" s="4"/>
       <c r="I79" s="5"/>
       <c r="O79" s="4"/>
-      <c r="P79" s="15"/>
-      <c r="Q79" s="15"/>
-      <c r="R79" s="15"/>
-      <c r="S79" s="15"/>
-      <c r="T79" s="15"/>
-      <c r="U79" s="15"/>
-      <c r="V79" s="15"/>
-      <c r="W79" s="15"/>
-      <c r="X79" s="15"/>
-      <c r="Y79" s="15"/>
-      <c r="Z79" s="15"/>
-      <c r="AA79" s="15"/>
-      <c r="AB79" s="15"/>
-      <c r="AC79" s="15"/>
-      <c r="AD79" s="15"/>
-      <c r="AE79" s="15"/>
-      <c r="AF79" s="15"/>
       <c r="AG79" s="5"/>
     </row>
     <row r="80" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
+        <v>108</v>
+      </c>
       <c r="I80" s="5"/>
       <c r="O80" s="4"/>
-      <c r="P80" s="15"/>
-      <c r="Q80" s="15"/>
-      <c r="R80" s="15"/>
-      <c r="S80" s="15"/>
-      <c r="T80" s="15"/>
-      <c r="U80" s="15"/>
-      <c r="V80" s="15"/>
-      <c r="W80" s="15"/>
-      <c r="X80" s="15"/>
-      <c r="Y80" s="15"/>
-      <c r="Z80" s="15"/>
-      <c r="AA80" s="15"/>
-      <c r="AB80" s="15"/>
-      <c r="AC80" s="15"/>
-      <c r="AD80" s="15"/>
-      <c r="AE80" s="15"/>
-      <c r="AF80" s="15"/>
       <c r="AG80" s="5"/>
     </row>
     <row r="81" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
+        <v>109</v>
+      </c>
       <c r="I81" s="5"/>
       <c r="O81" s="4"/>
-      <c r="P81" s="15"/>
-      <c r="Q81" s="15"/>
-      <c r="R81" s="15"/>
-      <c r="S81" s="15"/>
-      <c r="T81" s="15"/>
-      <c r="U81" s="15"/>
-      <c r="V81" s="15"/>
-      <c r="W81" s="15"/>
-      <c r="X81" s="15"/>
-      <c r="Y81" s="15"/>
-      <c r="Z81" s="15"/>
-      <c r="AA81" s="15"/>
-      <c r="AB81" s="15"/>
-      <c r="AC81" s="15"/>
-      <c r="AD81" s="15"/>
-      <c r="AE81" s="15"/>
-      <c r="AF81" s="15"/>
       <c r="AG81" s="5"/>
     </row>
     <row r="82" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="15"/>
-      <c r="F82" s="15"/>
-      <c r="G82" s="15"/>
-      <c r="H82" s="15"/>
+      <c r="B82" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I82" s="5"/>
       <c r="O82" s="4"/>
-      <c r="P82" s="15"/>
-      <c r="Q82" s="15"/>
-      <c r="R82" s="15"/>
-      <c r="S82" s="15"/>
-      <c r="T82" s="15"/>
-      <c r="U82" s="15"/>
-      <c r="V82" s="15"/>
-      <c r="W82" s="15"/>
-      <c r="X82" s="15"/>
-      <c r="Y82" s="15"/>
-      <c r="Z82" s="15"/>
-      <c r="AA82" s="15"/>
-      <c r="AB82" s="15"/>
-      <c r="AC82" s="15"/>
-      <c r="AD82" s="15"/>
-      <c r="AE82" s="15"/>
-      <c r="AF82" s="15"/>
       <c r="AG82" s="5"/>
     </row>
     <row r="83" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
+      <c r="B83" s="4"/>
       <c r="I83" s="5"/>
       <c r="O83" s="4"/>
-      <c r="P83" s="15"/>
-      <c r="Q83" s="15"/>
-      <c r="R83" s="15"/>
-      <c r="S83" s="15"/>
-      <c r="T83" s="15"/>
-      <c r="U83" s="15"/>
-      <c r="V83" s="15"/>
-      <c r="W83" s="15"/>
-      <c r="X83" s="15"/>
-      <c r="Y83" s="15"/>
-      <c r="Z83" s="15"/>
-      <c r="AA83" s="15"/>
-      <c r="AB83" s="15"/>
-      <c r="AC83" s="15"/>
-      <c r="AD83" s="15"/>
-      <c r="AE83" s="15"/>
-      <c r="AF83" s="15"/>
       <c r="AG83" s="5"/>
     </row>
     <row r="84" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C84" s="15"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="15"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="15"/>
-      <c r="H84" s="15"/>
+        <v>110</v>
+      </c>
       <c r="I84" s="5"/>
       <c r="O84" s="4"/>
-      <c r="P84" s="15"/>
-      <c r="Q84" s="15"/>
-      <c r="R84" s="15"/>
-      <c r="S84" s="15"/>
-      <c r="T84" s="15"/>
-      <c r="U84" s="15"/>
-      <c r="V84" s="15"/>
-      <c r="W84" s="15"/>
-      <c r="X84" s="15"/>
-      <c r="Y84" s="15"/>
-      <c r="Z84" s="15"/>
-      <c r="AA84" s="15"/>
-      <c r="AB84" s="15"/>
-      <c r="AC84" s="15"/>
-      <c r="AD84" s="15"/>
-      <c r="AE84" s="15"/>
-      <c r="AF84" s="15"/>
       <c r="AG84" s="5"/>
     </row>
     <row r="85" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="15"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="15"/>
-      <c r="H85" s="15"/>
+        <v>111</v>
+      </c>
       <c r="I85" s="5"/>
       <c r="O85" s="4"/>
-      <c r="P85" s="15"/>
-      <c r="Q85" s="15"/>
-      <c r="R85" s="15"/>
-      <c r="S85" s="15"/>
-      <c r="T85" s="15"/>
-      <c r="U85" s="15"/>
-      <c r="V85" s="15"/>
-      <c r="W85" s="15"/>
-      <c r="X85" s="15"/>
-      <c r="Y85" s="15"/>
-      <c r="Z85" s="15"/>
-      <c r="AA85" s="15"/>
-      <c r="AB85" s="15"/>
-      <c r="AC85" s="15"/>
-      <c r="AD85" s="15"/>
-      <c r="AE85" s="15"/>
-      <c r="AF85" s="15"/>
       <c r="AG85" s="5"/>
     </row>
     <row r="86" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B86" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="15"/>
-      <c r="F86" s="15"/>
-      <c r="G86" s="15"/>
-      <c r="H86" s="15"/>
+        <v>94</v>
+      </c>
       <c r="I86" s="5"/>
       <c r="O86" s="4"/>
-      <c r="P86" s="15"/>
-      <c r="Q86" s="15"/>
-      <c r="R86" s="15"/>
-      <c r="S86" s="15"/>
-      <c r="T86" s="15"/>
-      <c r="U86" s="15"/>
-      <c r="V86" s="15"/>
-      <c r="W86" s="15"/>
-      <c r="X86" s="15"/>
-      <c r="Y86" s="15"/>
-      <c r="Z86" s="15"/>
-      <c r="AA86" s="15"/>
-      <c r="AB86" s="15"/>
-      <c r="AC86" s="15"/>
-      <c r="AD86" s="15"/>
-      <c r="AE86" s="15"/>
-      <c r="AF86" s="15"/>
       <c r="AG86" s="5"/>
     </row>
     <row r="87" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="15"/>
-      <c r="F87" s="15"/>
-      <c r="G87" s="15"/>
-      <c r="H87" s="15"/>
+      <c r="B87" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="I87" s="5"/>
       <c r="O87" s="4"/>
-      <c r="P87" s="15"/>
-      <c r="Q87" s="15"/>
-      <c r="R87" s="15"/>
-      <c r="S87" s="15"/>
-      <c r="T87" s="15"/>
-      <c r="U87" s="15"/>
-      <c r="V87" s="15"/>
-      <c r="W87" s="15"/>
-      <c r="X87" s="15"/>
-      <c r="Y87" s="15"/>
-      <c r="Z87" s="15"/>
-      <c r="AA87" s="15"/>
-      <c r="AB87" s="15"/>
-      <c r="AC87" s="15"/>
-      <c r="AD87" s="15"/>
-      <c r="AE87" s="15"/>
-      <c r="AF87" s="15"/>
       <c r="AG87" s="5"/>
     </row>
     <row r="88" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C88" s="15"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="15"/>
-      <c r="F88" s="15"/>
-      <c r="G88" s="15"/>
-      <c r="H88" s="15"/>
+      <c r="B88" s="4"/>
       <c r="I88" s="5"/>
       <c r="O88" s="4"/>
-      <c r="P88" s="15"/>
-      <c r="Q88" s="15"/>
-      <c r="R88" s="15"/>
-      <c r="S88" s="15"/>
-      <c r="T88" s="15"/>
-      <c r="U88" s="15"/>
-      <c r="V88" s="15"/>
-      <c r="W88" s="15"/>
-      <c r="X88" s="15"/>
-      <c r="Y88" s="15"/>
-      <c r="Z88" s="15"/>
-      <c r="AA88" s="15"/>
-      <c r="AB88" s="15"/>
-      <c r="AC88" s="15"/>
-      <c r="AD88" s="15"/>
-      <c r="AE88" s="15"/>
-      <c r="AF88" s="15"/>
       <c r="AG88" s="5"/>
     </row>
     <row r="89" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15"/>
-      <c r="F89" s="15"/>
-      <c r="G89" s="15"/>
-      <c r="H89" s="15"/>
+        <v>112</v>
+      </c>
       <c r="I89" s="5"/>
       <c r="O89" s="4"/>
-      <c r="P89" s="15"/>
-      <c r="Q89" s="15"/>
-      <c r="R89" s="15"/>
-      <c r="S89" s="15"/>
-      <c r="T89" s="15"/>
-      <c r="U89" s="15"/>
-      <c r="V89" s="15"/>
-      <c r="W89" s="15"/>
-      <c r="X89" s="15"/>
-      <c r="Y89" s="15"/>
-      <c r="Z89" s="15"/>
-      <c r="AA89" s="15"/>
-      <c r="AB89" s="15"/>
-      <c r="AC89" s="15"/>
-      <c r="AD89" s="15"/>
-      <c r="AE89" s="15"/>
-      <c r="AF89" s="15"/>
       <c r="AG89" s="5"/>
     </row>
     <row r="90" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B90" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="15"/>
-      <c r="H90" s="15"/>
+        <v>115</v>
+      </c>
       <c r="I90" s="5"/>
       <c r="O90" s="4"/>
-      <c r="P90" s="15"/>
-      <c r="Q90" s="15"/>
-      <c r="R90" s="15"/>
-      <c r="S90" s="15"/>
-      <c r="T90" s="15"/>
-      <c r="U90" s="15"/>
-      <c r="V90" s="15"/>
-      <c r="W90" s="15"/>
-      <c r="X90" s="15"/>
-      <c r="Y90" s="15"/>
-      <c r="Z90" s="15"/>
-      <c r="AA90" s="15"/>
-      <c r="AB90" s="15"/>
-      <c r="AC90" s="15"/>
-      <c r="AD90" s="15"/>
-      <c r="AE90" s="15"/>
-      <c r="AF90" s="15"/>
       <c r="AG90" s="5"/>
     </row>
     <row r="91" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B91" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C91" s="15"/>
-      <c r="D91" s="15"/>
-      <c r="E91" s="15"/>
-      <c r="F91" s="15"/>
-      <c r="G91" s="15"/>
-      <c r="H91" s="15"/>
+        <v>109</v>
+      </c>
       <c r="I91" s="5"/>
       <c r="O91" s="4"/>
-      <c r="P91" s="15"/>
-      <c r="Q91" s="15"/>
-      <c r="R91" s="15"/>
-      <c r="S91" s="15"/>
-      <c r="T91" s="15"/>
-      <c r="U91" s="15"/>
-      <c r="V91" s="15"/>
-      <c r="W91" s="15"/>
-      <c r="X91" s="15"/>
-      <c r="Y91" s="15"/>
-      <c r="Z91" s="15"/>
-      <c r="AA91" s="15"/>
-      <c r="AB91" s="15"/>
-      <c r="AC91" s="15"/>
-      <c r="AD91" s="15"/>
-      <c r="AE91" s="15"/>
-      <c r="AF91" s="15"/>
       <c r="AG91" s="5"/>
     </row>
     <row r="92" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I92" s="5"/>
+      <c r="O92" s="4"/>
+      <c r="AG92" s="5"/>
+    </row>
+    <row r="93" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B93" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
-      <c r="H92" s="7"/>
-      <c r="I92" s="8"/>
-      <c r="O92" s="4"/>
-      <c r="P92" s="15"/>
-      <c r="Q92" s="15"/>
-      <c r="R92" s="15"/>
-      <c r="S92" s="15"/>
-      <c r="T92" s="15"/>
-      <c r="U92" s="15"/>
-      <c r="V92" s="15"/>
-      <c r="W92" s="15"/>
-      <c r="X92" s="15"/>
-      <c r="Y92" s="15"/>
-      <c r="Z92" s="15"/>
-      <c r="AA92" s="15"/>
-      <c r="AB92" s="15"/>
-      <c r="AC92" s="15"/>
-      <c r="AD92" s="15"/>
-      <c r="AE92" s="15"/>
-      <c r="AF92" s="15"/>
-      <c r="AG92" s="5"/>
-    </row>
-    <row r="93" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
+      <c r="I93" s="8"/>
       <c r="O93" s="4"/>
-      <c r="P93" s="15"/>
-      <c r="Q93" s="15"/>
-      <c r="R93" s="15"/>
-      <c r="S93" s="15"/>
-      <c r="T93" s="15"/>
-      <c r="U93" s="15"/>
-      <c r="V93" s="15"/>
-      <c r="W93" s="15"/>
-      <c r="X93" s="15"/>
-      <c r="Y93" s="15"/>
-      <c r="Z93" s="15"/>
-      <c r="AA93" s="15"/>
-      <c r="AB93" s="15"/>
-      <c r="AC93" s="15"/>
-      <c r="AD93" s="15"/>
-      <c r="AE93" s="15"/>
-      <c r="AF93" s="15"/>
       <c r="AG93" s="5"/>
     </row>
     <row r="94" spans="2:33" x14ac:dyDescent="0.25">
       <c r="O94" s="4"/>
-      <c r="P94" s="15"/>
-      <c r="Q94" s="15"/>
-      <c r="R94" s="15"/>
-      <c r="S94" s="15"/>
-      <c r="T94" s="15"/>
-      <c r="U94" s="15"/>
-      <c r="V94" s="15"/>
-      <c r="W94" s="15"/>
-      <c r="X94" s="15"/>
-      <c r="Y94" s="15"/>
-      <c r="Z94" s="15"/>
-      <c r="AA94" s="15"/>
-      <c r="AB94" s="15"/>
-      <c r="AC94" s="15"/>
-      <c r="AD94" s="15"/>
-      <c r="AE94" s="15"/>
-      <c r="AF94" s="15"/>
       <c r="AG94" s="5"/>
     </row>
     <row r="95" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="O95" s="6"/>
-      <c r="P95" s="7"/>
-      <c r="Q95" s="7"/>
-      <c r="R95" s="7"/>
-      <c r="S95" s="7"/>
-      <c r="T95" s="7"/>
-      <c r="U95" s="7"/>
-      <c r="V95" s="7"/>
-      <c r="W95" s="7"/>
-      <c r="X95" s="7"/>
-      <c r="Y95" s="7"/>
-      <c r="Z95" s="7"/>
-      <c r="AA95" s="7"/>
-      <c r="AB95" s="7"/>
-      <c r="AC95" s="7"/>
-      <c r="AD95" s="7"/>
-      <c r="AE95" s="7"/>
-      <c r="AF95" s="7"/>
-      <c r="AG95" s="8"/>
+      <c r="O95" s="4"/>
+      <c r="AG95" s="5"/>
+    </row>
+    <row r="96" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="O96" s="6"/>
+      <c r="P96" s="7"/>
+      <c r="Q96" s="7"/>
+      <c r="R96" s="7"/>
+      <c r="S96" s="7"/>
+      <c r="T96" s="7"/>
+      <c r="U96" s="7"/>
+      <c r="V96" s="7"/>
+      <c r="W96" s="7"/>
+      <c r="X96" s="7"/>
+      <c r="Y96" s="7"/>
+      <c r="Z96" s="7"/>
+      <c r="AA96" s="7"/>
+      <c r="AB96" s="7"/>
+      <c r="AC96" s="7"/>
+      <c r="AD96" s="7"/>
+      <c r="AE96" s="7"/>
+      <c r="AF96" s="7"/>
+      <c r="AG96" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6398F4F3-3A93-4EE8-9246-C0D41AE3E1CB}">
+  <dimension ref="A2:K50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="D15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="D16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="5"/>
+      <c r="J31" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="5"/>
+      <c r="J43" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Map Datatype - Collections in Apex
</commit_message>
<xml_diff>
--- a/me/2.Apex-Fundamentals.xlsx
+++ b/me/2.Apex-Fundamentals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CD1B98-A41A-49CD-A1DB-146229C39C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441836D8-5030-4529-857D-C9537D5516D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hello World" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Adding Comments" sheetId="5" r:id="rId5"/>
     <sheet name="List Collections Datatype" sheetId="6" r:id="rId6"/>
     <sheet name="Set Collections Datatype" sheetId="7" r:id="rId7"/>
+    <sheet name="Map Collections Datatype" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="174">
   <si>
     <t>Mở Developer Console trên tab mới</t>
   </si>
@@ -538,6 +539,108 @@
   </si>
   <si>
     <t>Xóa 1 item nên còn 5 item</t>
+  </si>
+  <si>
+    <t>8.map-collection-datatype.txt</t>
+  </si>
+  <si>
+    <t>salesforce\2.Apex-Fundamentals\8.map-collection-datatype.txt</t>
+  </si>
+  <si>
+    <t>Map&lt;Integer, String&gt; class2020 = new Map&lt;Integer, String&gt;();</t>
+  </si>
+  <si>
+    <t>// add a new student/item</t>
+  </si>
+  <si>
+    <t>class2020.put(11008890, 'Manish');</t>
+  </si>
+  <si>
+    <t>System.debug(class2020);</t>
+  </si>
+  <si>
+    <t>class2020.put(11008891, 'Harry');</t>
+  </si>
+  <si>
+    <t>class2020.put(11008892, 'Rick');</t>
+  </si>
+  <si>
+    <t>class2020.put(11008893, 'Bill');</t>
+  </si>
+  <si>
+    <t>class2020.put(11008894, 'Bill');</t>
+  </si>
+  <si>
+    <t>//update/override value</t>
+  </si>
+  <si>
+    <t>class2020.put(11008894, 'Skywalker');</t>
+  </si>
+  <si>
+    <t>// get a value</t>
+  </si>
+  <si>
+    <t>System.debug(class2020.get(11008892));</t>
+  </si>
+  <si>
+    <t>// remove an item from map</t>
+  </si>
+  <si>
+    <t>class2020.remove(11008893);</t>
+  </si>
+  <si>
+    <t>// get all the keys</t>
+  </si>
+  <si>
+    <t>Set&lt;Integer&gt; rollNumber = class2020.keySet();</t>
+  </si>
+  <si>
+    <t>// get all the values</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt; students = class2020.values();</t>
+  </si>
+  <si>
+    <t>System.debug(students);</t>
+  </si>
+  <si>
+    <t>// check if map has the key</t>
+  </si>
+  <si>
+    <t>System.debug(class2020.containsKey(11008892));</t>
+  </si>
+  <si>
+    <t>System.debug(class2020.containsKey(11008893));</t>
+  </si>
+  <si>
+    <t>Cũng giống với List và Set thì Map cũng lưu các giá trị Collection nhưng Map lưu data ở dạng key và value</t>
+  </si>
+  <si>
+    <t>Phần tử có key là 11008893 đã được xóa nên ko còn tồn tại</t>
+  </si>
+  <si>
+    <t>value Bill được update thành Skywalker</t>
+  </si>
+  <si>
+    <t>Cũng giống như Set thì Map cũng ko dùng index mà Map dùng key và value</t>
+  </si>
+  <si>
+    <t>Về cấu trúc dữ liệu của keySet() trả về</t>
+  </si>
+  <si>
+    <t>cũng là kiểu Set(ko duplicate value và</t>
+  </si>
+  <si>
+    <t>unordered)</t>
+  </si>
+  <si>
+    <t>values của Map được lưu dạng List(value</t>
+  </si>
+  <si>
+    <t>có thể duplicate)</t>
+  </si>
+  <si>
+    <t>value thì có thể duplicate nhưng key thì ko thể duplicate(key đóng vai trò giống như mã số sinh viên, value đóng vai trò là name của sv)</t>
   </si>
 </sst>
 </file>
@@ -666,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -687,7 +790,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2617,13 +2719,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>193860</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>94130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>468679</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>122059</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2661,13 +2763,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>168087</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>56030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>510986</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>48555</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2705,13 +2807,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>549088</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>493059</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2758,13 +2860,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>56031</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>89648</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>313766</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2802,13 +2904,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>56029</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>56030</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2855,13 +2957,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>246529</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>145676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>22412</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>156882</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3087,6 +3189,779 @@
         <a:xfrm>
           <a:off x="1524000" y="7381875"/>
           <a:ext cx="809625" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>274602</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>104057</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7C8E0E4-031B-989D-049B-DBE4DF9F3CDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8020050" y="3886200"/>
+          <a:ext cx="12980952" cy="5742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6934F90-9796-6222-E906-1852924CAE15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1524000" y="6457950"/>
+          <a:ext cx="9525" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCDCEB14-06AA-AC99-F00B-F4836AB6F359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2733675" y="6229350"/>
+          <a:ext cx="11772900" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B280BC68-3AF9-75CD-3D51-4C38D1D6A897}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1619250" y="5486400"/>
+          <a:ext cx="1038225" cy="2409825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18397C98-E6BE-3536-9838-F408EEA4D5E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3009900" y="6419850"/>
+          <a:ext cx="7610475" cy="1495425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D79448E5-1DA9-A36D-22A3-EDA4D67CF573}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1781175" y="8534400"/>
+          <a:ext cx="1123950" cy="2428875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C19E43-82C0-237B-D7F9-2E72E0C8316A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3533775" y="7477125"/>
+          <a:ext cx="7134225" cy="3495675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>46343</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123463</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5BED7FA-D39C-5B65-C8EC-9EDC1013E2A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="2943225"/>
+          <a:ext cx="10257143" cy="2895238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92D1764B-D34E-B54A-1BB1-83688817A20D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="12715875"/>
+          <a:ext cx="5362575" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB855A1F-11C9-367E-1942-FF934EF30B5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2305050" y="10248900"/>
+          <a:ext cx="8324850" cy="2600325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{846C4275-CE4C-1DC5-6C5F-A25E4610B12E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="13506450"/>
+          <a:ext cx="6477000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02609242-FB7D-5C7F-AF61-96D26AA915CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2133600" y="10439400"/>
+          <a:ext cx="8486775" cy="3200400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>503642</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114113</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD10571C-29AF-A5FB-A6BF-891F38162281}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="790575" y="1095375"/>
+          <a:ext cx="9466667" cy="1495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DB80CA1-CBD5-D28F-035C-E3D682A556FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1343025" y="561975"/>
+          <a:ext cx="4267200" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE3C2777-3F73-7C7E-8C00-EF1EC8530C87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2105025" y="542925"/>
+          <a:ext cx="5734050" cy="1524000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5702,7 +6577,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>116</v>
       </c>
       <c r="C3" s="2"/>
@@ -7304,85 +8179,724 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC5A17F-325A-41A3-9954-AF1931AC7357}">
-  <dimension ref="A2:AG96"/>
+  <dimension ref="A2:AG97"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="O39" s="1"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
-      <c r="AF39" s="2"/>
-      <c r="AG39" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="5"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="5"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="5"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="5"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="5"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="8"/>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="O40" s="4"/>
-      <c r="AG40" s="5"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="3"/>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="O41" s="4"/>
       <c r="AG41" s="5"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="3"/>
+      <c r="A42" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="O42" s="4"/>
       <c r="AG42" s="5"/>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="5"/>
+      <c r="B43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="3"/>
       <c r="O43" s="4"/>
       <c r="AG43" s="5"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
-      <c r="D44" t="s">
-        <v>12</v>
+      <c r="C44" t="s">
+        <v>11</v>
       </c>
       <c r="F44" s="5"/>
       <c r="O44" s="4"/>
@@ -7391,7 +8905,7 @@
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="D45" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F45" s="5"/>
       <c r="O45" s="4"/>
@@ -7400,7 +8914,7 @@
     <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="D46" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="F46" s="5"/>
       <c r="O46" s="4"/>
@@ -7409,7 +8923,7 @@
     <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="F47" s="5"/>
       <c r="O47" s="4"/>
@@ -7418,7 +8932,7 @@
     <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="D48" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F48" s="5"/>
       <c r="O48" s="4"/>
@@ -7426,29 +8940,34 @@
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
-      <c r="D49" s="10" t="s">
-        <v>92</v>
+      <c r="D49" t="s">
+        <v>81</v>
       </c>
       <c r="F49" s="5"/>
-      <c r="G49" t="s">
-        <v>17</v>
-      </c>
-      <c r="H49" t="s">
-        <v>16</v>
-      </c>
       <c r="O49" s="4"/>
       <c r="AG49" s="5"/>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B50" s="6"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="8"/>
+      <c r="B50" s="4"/>
+      <c r="D50" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" t="s">
+        <v>16</v>
+      </c>
       <c r="O50" s="4"/>
       <c r="AG50" s="5"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
       <c r="O51" s="4"/>
       <c r="AG51" s="5"/>
     </row>
@@ -7457,101 +8976,97 @@
       <c r="AG52" s="5"/>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>91</v>
-      </c>
       <c r="O53" s="4"/>
       <c r="AG53" s="5"/>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="3"/>
+      <c r="A54" t="s">
+        <v>91</v>
+      </c>
       <c r="O54" s="4"/>
       <c r="AG54" s="5"/>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I55" s="5"/>
+      <c r="B55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="3"/>
       <c r="O55" s="4"/>
       <c r="AG55" s="5"/>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I56" s="5"/>
       <c r="O56" s="4"/>
       <c r="AG56" s="5"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="B57" s="4"/>
       <c r="I57" s="5"/>
-      <c r="J57" t="s">
-        <v>17</v>
-      </c>
-      <c r="K57" t="s">
-        <v>113</v>
-      </c>
       <c r="O57" s="4"/>
       <c r="AG57" s="5"/>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I58" s="5"/>
+      <c r="J58" t="s">
+        <v>17</v>
+      </c>
+      <c r="K58" t="s">
+        <v>113</v>
+      </c>
       <c r="O58" s="4"/>
       <c r="AG58" s="5"/>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I59" s="5"/>
       <c r="O59" s="4"/>
       <c r="AG59" s="5"/>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
+      <c r="B60" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="I60" s="5"/>
       <c r="O60" s="4"/>
       <c r="AG60" s="5"/>
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="B61" s="4"/>
       <c r="I61" s="5"/>
       <c r="O61" s="4"/>
       <c r="AG61" s="5"/>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
+      <c r="B62" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I62" s="5"/>
       <c r="O62" s="4"/>
       <c r="AG62" s="5"/>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="B63" s="4"/>
       <c r="I63" s="5"/>
       <c r="O63" s="4"/>
       <c r="AG63" s="5"/>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I64" s="5"/>
       <c r="O64" s="4"/>
@@ -7559,7 +9074,7 @@
     </row>
     <row r="65" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I65" s="5"/>
       <c r="O65" s="4"/>
@@ -7567,93 +9082,93 @@
     </row>
     <row r="66" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I66" s="5"/>
       <c r="O66" s="4"/>
       <c r="AG66" s="5"/>
     </row>
     <row r="67" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B67" s="4"/>
+      <c r="B67" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="I67" s="5"/>
       <c r="O67" s="4"/>
       <c r="AG67" s="5"/>
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>102</v>
-      </c>
+      <c r="B68" s="4"/>
       <c r="I68" s="5"/>
       <c r="O68" s="4"/>
       <c r="AG68" s="5"/>
     </row>
     <row r="69" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I69" s="5"/>
-      <c r="J69" t="s">
-        <v>17</v>
-      </c>
-      <c r="K69" t="s">
-        <v>120</v>
-      </c>
       <c r="O69" s="4"/>
       <c r="AG69" s="5"/>
     </row>
     <row r="70" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="I70" s="5"/>
+      <c r="J70" t="s">
+        <v>17</v>
+      </c>
       <c r="K70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O70" s="4"/>
       <c r="AG70" s="5"/>
     </row>
     <row r="71" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B71" s="4"/>
+      <c r="B71" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I71" s="5"/>
       <c r="K71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O71" s="4"/>
       <c r="AG71" s="5"/>
     </row>
     <row r="72" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="B72" s="4"/>
       <c r="I72" s="5"/>
+      <c r="K72" t="s">
+        <v>122</v>
+      </c>
       <c r="O72" s="4"/>
       <c r="AG72" s="5"/>
     </row>
     <row r="73" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I73" s="5"/>
       <c r="O73" s="4"/>
       <c r="AG73" s="5"/>
     </row>
     <row r="74" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
+      <c r="B74" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="I74" s="5"/>
       <c r="O74" s="4"/>
       <c r="AG74" s="5"/>
     </row>
     <row r="75" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="B75" s="4"/>
       <c r="I75" s="5"/>
       <c r="O75" s="4"/>
       <c r="AG75" s="5"/>
     </row>
     <row r="76" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I76" s="5"/>
       <c r="O76" s="4"/>
@@ -7661,7 +9176,7 @@
     </row>
     <row r="77" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="I77" s="5"/>
       <c r="O77" s="4"/>
@@ -7669,29 +9184,29 @@
     </row>
     <row r="78" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I78" s="5"/>
       <c r="O78" s="4"/>
       <c r="AG78" s="5"/>
     </row>
     <row r="79" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B79" s="4"/>
+      <c r="B79" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="I79" s="5"/>
       <c r="O79" s="4"/>
       <c r="AG79" s="5"/>
     </row>
     <row r="80" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="B80" s="4"/>
       <c r="I80" s="5"/>
       <c r="O80" s="4"/>
       <c r="AG80" s="5"/>
     </row>
     <row r="81" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I81" s="5"/>
       <c r="O81" s="4"/>
@@ -7699,29 +9214,29 @@
     </row>
     <row r="82" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="I82" s="5"/>
       <c r="O82" s="4"/>
       <c r="AG82" s="5"/>
     </row>
     <row r="83" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B83" s="4"/>
+      <c r="B83" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I83" s="5"/>
       <c r="O83" s="4"/>
       <c r="AG83" s="5"/>
     </row>
     <row r="84" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="B84" s="4"/>
       <c r="I84" s="5"/>
       <c r="O84" s="4"/>
       <c r="AG84" s="5"/>
     </row>
     <row r="85" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I85" s="5"/>
       <c r="O85" s="4"/>
@@ -7729,7 +9244,7 @@
     </row>
     <row r="86" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B86" s="4" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="I86" s="5"/>
       <c r="O86" s="4"/>
@@ -7737,29 +9252,29 @@
     </row>
     <row r="87" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B87" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I87" s="5"/>
       <c r="O87" s="4"/>
       <c r="AG87" s="5"/>
     </row>
     <row r="88" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
+      <c r="B88" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="I88" s="5"/>
       <c r="O88" s="4"/>
       <c r="AG88" s="5"/>
     </row>
     <row r="89" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="B89" s="4"/>
       <c r="I89" s="5"/>
       <c r="O89" s="4"/>
       <c r="AG89" s="5"/>
     </row>
     <row r="90" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B90" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I90" s="5"/>
       <c r="O90" s="4"/>
@@ -7767,7 +9282,7 @@
     </row>
     <row r="91" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B91" s="4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="I91" s="5"/>
       <c r="O91" s="4"/>
@@ -7775,27 +9290,31 @@
     </row>
     <row r="92" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="I92" s="5"/>
       <c r="O92" s="4"/>
       <c r="AG92" s="5"/>
     </row>
     <row r="93" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B93" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="8"/>
+      <c r="B93" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I93" s="5"/>
       <c r="O93" s="4"/>
       <c r="AG93" s="5"/>
     </row>
     <row r="94" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B94" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="8"/>
       <c r="O94" s="4"/>
       <c r="AG94" s="5"/>
     </row>
@@ -7804,25 +9323,29 @@
       <c r="AG95" s="5"/>
     </row>
     <row r="96" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="O96" s="6"/>
-      <c r="P96" s="7"/>
-      <c r="Q96" s="7"/>
-      <c r="R96" s="7"/>
-      <c r="S96" s="7"/>
-      <c r="T96" s="7"/>
-      <c r="U96" s="7"/>
-      <c r="V96" s="7"/>
-      <c r="W96" s="7"/>
-      <c r="X96" s="7"/>
-      <c r="Y96" s="7"/>
-      <c r="Z96" s="7"/>
-      <c r="AA96" s="7"/>
-      <c r="AB96" s="7"/>
-      <c r="AC96" s="7"/>
-      <c r="AD96" s="7"/>
-      <c r="AE96" s="7"/>
-      <c r="AF96" s="7"/>
-      <c r="AG96" s="8"/>
+      <c r="O96" s="4"/>
+      <c r="AG96" s="5"/>
+    </row>
+    <row r="97" spans="15:33" x14ac:dyDescent="0.25">
+      <c r="O97" s="6"/>
+      <c r="P97" s="7"/>
+      <c r="Q97" s="7"/>
+      <c r="R97" s="7"/>
+      <c r="S97" s="7"/>
+      <c r="T97" s="7"/>
+      <c r="U97" s="7"/>
+      <c r="V97" s="7"/>
+      <c r="W97" s="7"/>
+      <c r="X97" s="7"/>
+      <c r="Y97" s="7"/>
+      <c r="Z97" s="7"/>
+      <c r="AA97" s="7"/>
+      <c r="AB97" s="7"/>
+      <c r="AC97" s="7"/>
+      <c r="AD97" s="7"/>
+      <c r="AE97" s="7"/>
+      <c r="AF97" s="7"/>
+      <c r="AG97" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7834,8 +9357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6398F4F3-3A93-4EE8-9246-C0D41AE3E1CB}">
   <dimension ref="A2:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7913,7 +9436,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
-      <c r="D15" s="16" t="s">
+      <c r="D15" t="s">
         <v>92</v>
       </c>
       <c r="F15" s="5"/>
@@ -7959,114 +9482,54 @@
       <c r="B22" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
       <c r="I31" s="5"/>
       <c r="J31" t="s">
         <v>17</v>
@@ -8079,138 +9542,66 @@
       <c r="B32" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
       <c r="I43" s="5"/>
       <c r="J43" t="s">
         <v>17</v>
@@ -8221,70 +9612,34 @@
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -8303,4 +9658,559 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617CB9F7-276E-4C30-A5F6-F1811BB9A590}">
+  <dimension ref="A2:J86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="D38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="D42" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="D43" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="D44" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="5"/>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="4"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="5"/>
+      <c r="I66" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="5"/>
+      <c r="I77" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="5"/>
+      <c r="J78" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="5"/>
+      <c r="J79" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="5"/>
+      <c r="I81" t="s">
+        <v>17</v>
+      </c>
+      <c r="J81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="5"/>
+      <c r="J82" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="4"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B86" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="8"/>
+      <c r="I86" t="s">
+        <v>17</v>
+      </c>
+      <c r="J86" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>